<commit_message>
modified:   .gitignore 	modified:   input/Stammdaten_ISY.xml 	new file:   input/bauwerk_error.txt 	modified:   main.py 	modified:   massen_haltungen.csv 	modified:   massen_haltungen.xlsx 	modified:   massen_leitung.csv 	new file:   massen_schacht.csv 	modified:   massen_util/__inti__.py 	modified:   massen_util/csv_creator.py 	modified:   massen_util/merge_elements.py 	modified:   massen_util/pyexcel.py 	new file:   sorted_data.csv 	modified:   xml_parser/anschlusspunkt.py 	modified:   xml_parser/bauwerk.py 	modified:   xml_parser/flaechen.py 	modified:   xml_parser/haltung.py 	modified:   xml_parser/leitung.py 	modified:   xml_parser/parse_all.py 	modified:   xml_parser/schacht.py
</commit_message>
<xml_diff>
--- a/massen_haltungen.xlsx
+++ b/massen_haltungen.xlsx
@@ -1474,7 +1474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W129"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
@@ -1879,28 +1879,28 @@
     <row r="7" ht="14.65" customHeight="1" s="45">
       <c r="A7" s="67" t="inlineStr">
         <is>
-          <t>R1234</t>
+          <t>A057c</t>
         </is>
       </c>
       <c r="B7" s="67" t="inlineStr">
         <is>
-          <t>R1235</t>
+          <t>A057a</t>
         </is>
       </c>
       <c r="C7" s="68" t="n">
-        <v>12</v>
+        <v>211.07</v>
       </c>
       <c r="D7" s="68" t="n">
-        <v>11</v>
+        <v>211.237</v>
       </c>
       <c r="E7" s="68" t="n">
-        <v>10</v>
+        <v>210.77</v>
       </c>
       <c r="F7" s="69" t="n">
-        <v>8</v>
+        <v>210.757</v>
       </c>
       <c r="G7" s="68" t="n">
-        <v>6.46</v>
+        <v>5.78</v>
       </c>
       <c r="H7" s="70" t="n">
         <v>1.1</v>
@@ -1918,7 +1918,7 @@
         <v/>
       </c>
       <c r="L7" s="73" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="M7" s="74" t="n">
         <v>0.02</v>
@@ -1961,13 +1961,31 @@
       </c>
     </row>
     <row r="8" ht="14.65" customHeight="1" s="45">
-      <c r="A8" s="67" t="n"/>
-      <c r="B8" s="73" t="n"/>
-      <c r="C8" s="68" t="n"/>
-      <c r="D8" s="68" t="n"/>
-      <c r="E8" s="68" t="n"/>
-      <c r="F8" s="69" t="n"/>
-      <c r="G8" s="68" t="n"/>
+      <c r="A8" s="67" t="inlineStr">
+        <is>
+          <t>A057c</t>
+        </is>
+      </c>
+      <c r="B8" s="73" t="inlineStr">
+        <is>
+          <t>A057d</t>
+        </is>
+      </c>
+      <c r="C8" s="68" t="n">
+        <v>211.07</v>
+      </c>
+      <c r="D8" s="68" t="n">
+        <v>208.76</v>
+      </c>
+      <c r="E8" s="68" t="n">
+        <v>210.77</v>
+      </c>
+      <c r="F8" s="69" t="n">
+        <v>208.52</v>
+      </c>
+      <c r="G8" s="68" t="n">
+        <v>7.85</v>
+      </c>
       <c r="H8" s="70" t="n">
         <v>1.1</v>
       </c>
@@ -1983,7 +2001,9 @@
         <f>J8+M8+0.1</f>
         <v/>
       </c>
-      <c r="L8" s="73" t="n"/>
+      <c r="L8" s="73" t="n">
+        <v>100</v>
+      </c>
       <c r="M8" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2018,15 +2038,38 @@
         <f>2*G8*(K8-O8+0.05)</f>
         <v/>
       </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="14.65" customHeight="1" s="45">
-      <c r="A9" s="76" t="n"/>
-      <c r="B9" s="73" t="n"/>
-      <c r="C9" s="68" t="n"/>
-      <c r="D9" s="68" t="n"/>
-      <c r="E9" s="68" t="n"/>
-      <c r="F9" s="69" t="n"/>
-      <c r="G9" s="77" t="n"/>
+      <c r="A9" s="76" t="inlineStr">
+        <is>
+          <t>BAPUE4002</t>
+        </is>
+      </c>
+      <c r="B9" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4003</t>
+        </is>
+      </c>
+      <c r="C9" s="68" t="n">
+        <v>212.87</v>
+      </c>
+      <c r="D9" s="68" t="n">
+        <v>212.87</v>
+      </c>
+      <c r="E9" s="68" t="n">
+        <v>211.46</v>
+      </c>
+      <c r="F9" s="69" t="n">
+        <v>210.6</v>
+      </c>
+      <c r="G9" s="77" t="n">
+        <v>24.84</v>
+      </c>
       <c r="H9" s="78" t="n">
         <v>1.1</v>
       </c>
@@ -2042,7 +2085,9 @@
         <f>J9+M9+0.1</f>
         <v/>
       </c>
-      <c r="L9" s="81" t="n"/>
+      <c r="L9" s="81" t="n">
+        <v>800</v>
+      </c>
       <c r="M9" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2077,15 +2122,38 @@
         <f>2*G9*(K9-O9+0.05)</f>
         <v/>
       </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="14.65" customHeight="1" s="45">
-      <c r="A10" s="67" t="n"/>
-      <c r="B10" s="73" t="n"/>
-      <c r="C10" s="68" t="n"/>
-      <c r="D10" s="68" t="n"/>
-      <c r="E10" s="68" t="n"/>
-      <c r="F10" s="69" t="n"/>
-      <c r="G10" s="68" t="n"/>
+      <c r="A10" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4003</t>
+        </is>
+      </c>
+      <c r="B10" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4004</t>
+        </is>
+      </c>
+      <c r="C10" s="68" t="n">
+        <v>212.87</v>
+      </c>
+      <c r="D10" s="68" t="n">
+        <v>212.72</v>
+      </c>
+      <c r="E10" s="68" t="n">
+        <v>210.6</v>
+      </c>
+      <c r="F10" s="69" t="n">
+        <v>210.45</v>
+      </c>
+      <c r="G10" s="68" t="n">
+        <v>5.79</v>
+      </c>
       <c r="H10" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2101,7 +2169,9 @@
         <f>J10+M10+0.1</f>
         <v/>
       </c>
-      <c r="L10" s="73" t="n"/>
+      <c r="L10" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M10" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2136,15 +2206,38 @@
         <f>2*G10*(K10-O10+0.05)</f>
         <v/>
       </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="14.65" customHeight="1" s="45">
-      <c r="A11" s="67" t="n"/>
-      <c r="B11" s="73" t="n"/>
-      <c r="C11" s="68" t="n"/>
-      <c r="D11" s="68" t="n"/>
-      <c r="E11" s="68" t="n"/>
-      <c r="F11" s="69" t="n"/>
-      <c r="G11" s="68" t="n"/>
+      <c r="A11" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4004</t>
+        </is>
+      </c>
+      <c r="B11" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4005</t>
+        </is>
+      </c>
+      <c r="C11" s="68" t="n">
+        <v>212.72</v>
+      </c>
+      <c r="D11" s="68" t="n">
+        <v>210.87</v>
+      </c>
+      <c r="E11" s="68" t="n">
+        <v>210.45</v>
+      </c>
+      <c r="F11" s="69" t="n">
+        <v>209.75</v>
+      </c>
+      <c r="G11" s="68" t="n">
+        <v>16.38</v>
+      </c>
       <c r="H11" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2160,7 +2253,9 @@
         <f>J11+M11+0.1</f>
         <v/>
       </c>
-      <c r="L11" s="73" t="n"/>
+      <c r="L11" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M11" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2195,15 +2290,38 @@
         <f>2*G11*(K11-O11+0.05)</f>
         <v/>
       </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="14.65" customHeight="1" s="45">
-      <c r="A12" s="67" t="n"/>
-      <c r="B12" s="73" t="n"/>
-      <c r="C12" s="68" t="n"/>
-      <c r="D12" s="68" t="n"/>
-      <c r="E12" s="68" t="n"/>
-      <c r="F12" s="69" t="n"/>
-      <c r="G12" s="68" t="n"/>
+      <c r="A12" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4005</t>
+        </is>
+      </c>
+      <c r="B12" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4012</t>
+        </is>
+      </c>
+      <c r="C12" s="68" t="n">
+        <v>210.87</v>
+      </c>
+      <c r="D12" s="68" t="n">
+        <v>210.36</v>
+      </c>
+      <c r="E12" s="68" t="n">
+        <v>209.75</v>
+      </c>
+      <c r="F12" s="69" t="n">
+        <v>208.83</v>
+      </c>
+      <c r="G12" s="68" t="n">
+        <v>13.91</v>
+      </c>
       <c r="H12" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2219,7 +2337,9 @@
         <f>J12+M12+0.1</f>
         <v/>
       </c>
-      <c r="L12" s="73" t="n"/>
+      <c r="L12" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M12" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2254,15 +2374,38 @@
         <f>2*G12*(K12-O12+0.05)</f>
         <v/>
       </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="14.65" customHeight="1" s="45">
-      <c r="A13" s="67" t="n"/>
-      <c r="B13" s="73" t="n"/>
-      <c r="C13" s="68" t="n"/>
-      <c r="D13" s="68" t="n"/>
-      <c r="E13" s="68" t="n"/>
-      <c r="F13" s="69" t="n"/>
-      <c r="G13" s="68" t="n"/>
+      <c r="A13" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4009</t>
+        </is>
+      </c>
+      <c r="B13" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4010</t>
+        </is>
+      </c>
+      <c r="C13" s="68" t="n">
+        <v>214.15</v>
+      </c>
+      <c r="D13" s="68" t="n">
+        <v>213.69</v>
+      </c>
+      <c r="E13" s="68" t="n">
+        <v>212.65</v>
+      </c>
+      <c r="F13" s="69" t="n">
+        <v>212.52</v>
+      </c>
+      <c r="G13" s="68" t="n">
+        <v>5.39</v>
+      </c>
       <c r="H13" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2278,7 +2421,9 @@
         <f>J13+M13+0.1</f>
         <v/>
       </c>
-      <c r="L13" s="73" t="n"/>
+      <c r="L13" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M13" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2313,15 +2458,38 @@
         <f>2*G13*(K13-O13+0.05)</f>
         <v/>
       </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="14.65" customHeight="1" s="45">
-      <c r="A14" s="67" t="n"/>
-      <c r="B14" s="73" t="n"/>
-      <c r="C14" s="68" t="n"/>
-      <c r="D14" s="68" t="n"/>
-      <c r="E14" s="68" t="n"/>
-      <c r="F14" s="69" t="n"/>
-      <c r="G14" s="68" t="n"/>
+      <c r="A14" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4010</t>
+        </is>
+      </c>
+      <c r="B14" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4002</t>
+        </is>
+      </c>
+      <c r="C14" s="68" t="n">
+        <v>213.69</v>
+      </c>
+      <c r="D14" s="68" t="n">
+        <v>212.87</v>
+      </c>
+      <c r="E14" s="68" t="n">
+        <v>212.52</v>
+      </c>
+      <c r="F14" s="69" t="n">
+        <v>211.46</v>
+      </c>
+      <c r="G14" s="68" t="n">
+        <v>8.17</v>
+      </c>
       <c r="H14" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2337,7 +2505,9 @@
         <f>J14+M14+0.1</f>
         <v/>
       </c>
-      <c r="L14" s="73" t="n"/>
+      <c r="L14" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M14" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2372,15 +2542,38 @@
         <f>2*G14*(K14-O14+0.05)</f>
         <v/>
       </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="14.65" customHeight="1" s="45">
-      <c r="A15" s="67" t="n"/>
-      <c r="B15" s="73" t="n"/>
-      <c r="C15" s="68" t="n"/>
-      <c r="D15" s="68" t="n"/>
-      <c r="E15" s="68" t="n"/>
-      <c r="F15" s="69" t="n"/>
-      <c r="G15" s="68" t="n"/>
+      <c r="A15" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4012</t>
+        </is>
+      </c>
+      <c r="B15" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4013</t>
+        </is>
+      </c>
+      <c r="C15" s="68" t="n">
+        <v>210.36</v>
+      </c>
+      <c r="D15" s="68" t="n">
+        <v>209.97</v>
+      </c>
+      <c r="E15" s="68" t="n">
+        <v>208.83</v>
+      </c>
+      <c r="F15" s="69" t="n">
+        <v>207.75</v>
+      </c>
+      <c r="G15" s="68" t="n">
+        <v>4.14</v>
+      </c>
       <c r="H15" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2396,7 +2589,9 @@
         <f>J15+M15+0.1</f>
         <v/>
       </c>
-      <c r="L15" s="73" t="n"/>
+      <c r="L15" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M15" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2431,15 +2626,38 @@
         <f>2*G15*(K15-O15+0.05)</f>
         <v/>
       </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="14.65" customHeight="1" s="45">
-      <c r="A16" s="67" t="n"/>
-      <c r="B16" s="73" t="n"/>
-      <c r="C16" s="68" t="n"/>
-      <c r="D16" s="68" t="n"/>
-      <c r="E16" s="68" t="n"/>
-      <c r="F16" s="69" t="n"/>
-      <c r="G16" s="68" t="n"/>
+      <c r="A16" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4013</t>
+        </is>
+      </c>
+      <c r="B16" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4014</t>
+        </is>
+      </c>
+      <c r="C16" s="68" t="n">
+        <v>209.97</v>
+      </c>
+      <c r="D16" s="68" t="n">
+        <v>208.41</v>
+      </c>
+      <c r="E16" s="68" t="n">
+        <v>207.75</v>
+      </c>
+      <c r="F16" s="69" t="n">
+        <v>206.67</v>
+      </c>
+      <c r="G16" s="68" t="n">
+        <v>47.21</v>
+      </c>
       <c r="H16" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2455,7 +2673,9 @@
         <f>J16+M16+0.1</f>
         <v/>
       </c>
-      <c r="L16" s="73" t="n"/>
+      <c r="L16" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M16" s="74" t="n">
         <v>0.02</v>
       </c>
@@ -2490,15 +2710,38 @@
         <f>2*G16*(K16-O16+0.05)</f>
         <v/>
       </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="14.65" customHeight="1" s="45">
-      <c r="A17" s="67" t="n"/>
-      <c r="B17" s="73" t="n"/>
-      <c r="C17" s="68" t="n"/>
-      <c r="D17" s="68" t="n"/>
-      <c r="E17" s="68" t="n"/>
-      <c r="F17" s="69" t="n"/>
-      <c r="G17" s="68" t="n"/>
+      <c r="A17" s="67" t="inlineStr">
+        <is>
+          <t>BAPUE4014</t>
+        </is>
+      </c>
+      <c r="B17" s="73" t="inlineStr">
+        <is>
+          <t>BAPUE4015AL</t>
+        </is>
+      </c>
+      <c r="C17" s="68" t="n">
+        <v>208.41</v>
+      </c>
+      <c r="D17" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="68" t="n">
+        <v>206.67</v>
+      </c>
+      <c r="F17" s="69" t="n">
+        <v>206.47</v>
+      </c>
+      <c r="G17" s="68" t="n">
+        <v>15.49</v>
+      </c>
       <c r="H17" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2514,7 +2757,9 @@
         <f>J17+M17+0.1</f>
         <v/>
       </c>
-      <c r="L17" s="73" t="n"/>
+      <c r="L17" s="73" t="n">
+        <v>800</v>
+      </c>
       <c r="M17" s="74" t="n">
         <v>0.03</v>
       </c>
@@ -2549,15 +2794,38 @@
         <f>2*G17*(K17-O17+0.05)</f>
         <v/>
       </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="14.65" customHeight="1" s="45">
-      <c r="A18" s="67" t="n"/>
-      <c r="B18" s="73" t="n"/>
-      <c r="C18" s="68" t="n"/>
-      <c r="D18" s="68" t="n"/>
-      <c r="E18" s="68" t="n"/>
-      <c r="F18" s="69" t="n"/>
-      <c r="G18" s="68" t="n"/>
+      <c r="A18" s="67" t="inlineStr">
+        <is>
+          <t>FIKTIV</t>
+        </is>
+      </c>
+      <c r="B18" s="73" t="inlineStr">
+        <is>
+          <t>1348.2</t>
+        </is>
+      </c>
+      <c r="C18" s="68" t="n">
+        <v>226</v>
+      </c>
+      <c r="D18" s="68" t="n">
+        <v>225.64</v>
+      </c>
+      <c r="E18" s="68" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="F18" s="69" t="n">
+        <v>223.98</v>
+      </c>
+      <c r="G18" s="68" t="n">
+        <v>17.21</v>
+      </c>
       <c r="H18" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2573,7 +2841,9 @@
         <f>J18+M18+0.1</f>
         <v/>
       </c>
-      <c r="L18" s="73" t="n"/>
+      <c r="L18" s="73" t="n">
+        <v>150</v>
+      </c>
       <c r="M18" s="74" t="n">
         <v>0.03</v>
       </c>
@@ -2608,15 +2878,38 @@
         <f>2*G18*(K18-O18+0.05)</f>
         <v/>
       </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="14.65" customHeight="1" s="45">
-      <c r="A19" s="67" t="n"/>
-      <c r="B19" s="73" t="n"/>
-      <c r="C19" s="68" t="n"/>
-      <c r="D19" s="68" t="n"/>
-      <c r="E19" s="68" t="n"/>
-      <c r="F19" s="69" t="n"/>
-      <c r="G19" s="68" t="n"/>
+      <c r="A19" s="67" t="inlineStr">
+        <is>
+          <t>HS-028</t>
+        </is>
+      </c>
+      <c r="B19" s="73" t="inlineStr">
+        <is>
+          <t>HS-027</t>
+        </is>
+      </c>
+      <c r="C19" s="68" t="n">
+        <v>207.68</v>
+      </c>
+      <c r="D19" s="68" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="E19" s="68" t="n">
+        <v>204.68</v>
+      </c>
+      <c r="F19" s="69" t="n">
+        <v>204.59</v>
+      </c>
+      <c r="G19" s="68" t="n">
+        <v>55.29</v>
+      </c>
       <c r="H19" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2632,7 +2925,9 @@
         <f>J19+M19+0.1</f>
         <v/>
       </c>
-      <c r="L19" s="73" t="n"/>
+      <c r="L19" s="73" t="n">
+        <v>500</v>
+      </c>
       <c r="M19" s="74" t="n">
         <v>0.03</v>
       </c>
@@ -2667,15 +2962,38 @@
         <f>2*G19*(K19-O19+0.05)</f>
         <v/>
       </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="14.65" customHeight="1" s="45">
-      <c r="A20" s="67" t="n"/>
-      <c r="B20" s="73" t="n"/>
-      <c r="C20" s="68" t="n"/>
-      <c r="D20" s="68" t="n"/>
-      <c r="E20" s="68" t="n"/>
-      <c r="F20" s="69" t="n"/>
-      <c r="G20" s="68" t="n"/>
+      <c r="A20" s="67" t="inlineStr">
+        <is>
+          <t>HS-029</t>
+        </is>
+      </c>
+      <c r="B20" s="73" t="inlineStr">
+        <is>
+          <t>HS-028</t>
+        </is>
+      </c>
+      <c r="C20" s="68" t="n">
+        <v>207.24</v>
+      </c>
+      <c r="D20" s="68" t="n">
+        <v>207.68</v>
+      </c>
+      <c r="E20" s="68" t="n">
+        <v>204.8</v>
+      </c>
+      <c r="F20" s="69" t="n">
+        <v>204.68</v>
+      </c>
+      <c r="G20" s="68" t="n">
+        <v>60.4</v>
+      </c>
       <c r="H20" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2691,7 +3009,9 @@
         <f>J20+M20+0.1</f>
         <v/>
       </c>
-      <c r="L20" s="73" t="n"/>
+      <c r="L20" s="73" t="n">
+        <v>500</v>
+      </c>
       <c r="M20" s="74" t="n">
         <v>0.03</v>
       </c>
@@ -2726,15 +3046,38 @@
         <f>2*G20*(K20-O20+0.05)</f>
         <v/>
       </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="14.65" customHeight="1" s="45">
-      <c r="A21" s="67" t="n"/>
-      <c r="B21" s="73" t="n"/>
-      <c r="C21" s="68" t="n"/>
-      <c r="D21" s="68" t="n"/>
-      <c r="E21" s="68" t="n"/>
-      <c r="F21" s="69" t="n"/>
-      <c r="G21" s="68" t="n"/>
+      <c r="A21" s="67" t="inlineStr">
+        <is>
+          <t>HS-030</t>
+        </is>
+      </c>
+      <c r="B21" s="73" t="inlineStr">
+        <is>
+          <t>HS-029</t>
+        </is>
+      </c>
+      <c r="C21" s="68" t="n">
+        <v>207.91</v>
+      </c>
+      <c r="D21" s="68" t="n">
+        <v>207.24</v>
+      </c>
+      <c r="E21" s="68" t="n">
+        <v>204.91</v>
+      </c>
+      <c r="F21" s="69" t="n">
+        <v>204.8</v>
+      </c>
+      <c r="G21" s="68" t="n">
+        <v>40.19</v>
+      </c>
       <c r="H21" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2750,7 +3093,9 @@
         <f>J21+M21+0.1</f>
         <v/>
       </c>
-      <c r="L21" s="73" t="n"/>
+      <c r="L21" s="73" t="n">
+        <v>500</v>
+      </c>
       <c r="M21" s="74" t="n">
         <v>0.03</v>
       </c>
@@ -2785,15 +3130,38 @@
         <f>2*G21*(K21-O21+0.05)</f>
         <v/>
       </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="14.65" customHeight="1" s="45">
-      <c r="A22" s="76" t="n"/>
-      <c r="B22" s="73" t="n"/>
-      <c r="C22" s="68" t="n"/>
-      <c r="D22" s="68" t="n"/>
-      <c r="E22" s="68" t="n"/>
-      <c r="F22" s="69" t="n"/>
-      <c r="G22" s="82" t="n"/>
+      <c r="A22" s="76" t="inlineStr">
+        <is>
+          <t>HS-031</t>
+        </is>
+      </c>
+      <c r="B22" s="73" t="inlineStr">
+        <is>
+          <t>HS-030</t>
+        </is>
+      </c>
+      <c r="C22" s="68" t="n">
+        <v>208.61</v>
+      </c>
+      <c r="D22" s="68" t="n">
+        <v>207.91</v>
+      </c>
+      <c r="E22" s="68" t="n">
+        <v>205.07</v>
+      </c>
+      <c r="F22" s="69" t="n">
+        <v>204.91</v>
+      </c>
+      <c r="G22" s="82" t="n">
+        <v>40.23</v>
+      </c>
       <c r="H22" s="78" t="n">
         <v>1.1</v>
       </c>
@@ -2809,7 +3177,9 @@
         <f>J22+M22+0.1</f>
         <v/>
       </c>
-      <c r="L22" s="81" t="n"/>
+      <c r="L22" s="81" t="n">
+        <v>480</v>
+      </c>
       <c r="M22" s="74" t="n">
         <v>0.03</v>
       </c>
@@ -2844,15 +3214,38 @@
         <f>2*G22*(K22-O22+0.05)</f>
         <v/>
       </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="14.65" customHeight="1" s="45">
-      <c r="A23" s="67" t="n"/>
-      <c r="B23" s="73" t="n"/>
-      <c r="C23" s="68" t="n"/>
-      <c r="D23" s="68" t="n"/>
-      <c r="E23" s="68" t="n"/>
-      <c r="F23" s="69" t="n"/>
-      <c r="G23" s="68" t="n"/>
+      <c r="A23" s="67" t="inlineStr">
+        <is>
+          <t>HS-032</t>
+        </is>
+      </c>
+      <c r="B23" s="73" t="inlineStr">
+        <is>
+          <t>HS-031</t>
+        </is>
+      </c>
+      <c r="C23" s="68" t="n">
+        <v>207.93</v>
+      </c>
+      <c r="D23" s="68" t="n">
+        <v>208.61</v>
+      </c>
+      <c r="E23" s="68" t="n">
+        <v>205.22</v>
+      </c>
+      <c r="F23" s="69" t="n">
+        <v>205.07</v>
+      </c>
+      <c r="G23" s="68" t="n">
+        <v>35.05</v>
+      </c>
       <c r="H23" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2868,7 +3261,9 @@
         <f>J23+M23+0.1</f>
         <v/>
       </c>
-      <c r="L23" s="73" t="n"/>
+      <c r="L23" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M23" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -2903,15 +3298,38 @@
         <f>2*G23*(K23-O23+0.05)</f>
         <v/>
       </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="14.65" customHeight="1" s="45">
-      <c r="A24" s="67" t="n"/>
-      <c r="B24" s="73" t="n"/>
-      <c r="C24" s="68" t="n"/>
-      <c r="D24" s="68" t="n"/>
-      <c r="E24" s="68" t="n"/>
-      <c r="F24" s="69" t="n"/>
-      <c r="G24" s="68" t="n"/>
+      <c r="A24" s="67" t="inlineStr">
+        <is>
+          <t>HS-033</t>
+        </is>
+      </c>
+      <c r="B24" s="73" t="inlineStr">
+        <is>
+          <t>HS-032</t>
+        </is>
+      </c>
+      <c r="C24" s="68" t="n">
+        <v>207.8</v>
+      </c>
+      <c r="D24" s="68" t="n">
+        <v>207.93</v>
+      </c>
+      <c r="E24" s="68" t="n">
+        <v>205.3</v>
+      </c>
+      <c r="F24" s="69" t="n">
+        <v>205.22</v>
+      </c>
+      <c r="G24" s="68" t="n">
+        <v>50.19</v>
+      </c>
       <c r="H24" s="70" t="n">
         <v>1.1</v>
       </c>
@@ -2927,7 +3345,9 @@
         <f>J24+M24+0.1</f>
         <v/>
       </c>
-      <c r="L24" s="73" t="n"/>
+      <c r="L24" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M24" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -2962,15 +3382,38 @@
         <f>2*G24*(K24-O24+0.05)</f>
         <v/>
       </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="14.65" customHeight="1" s="45">
-      <c r="A25" s="67" t="n"/>
-      <c r="B25" s="73" t="n"/>
-      <c r="C25" s="68" t="n"/>
-      <c r="D25" s="68" t="n"/>
-      <c r="E25" s="68" t="n"/>
-      <c r="F25" s="69" t="n"/>
-      <c r="G25" s="68" t="n"/>
+      <c r="A25" s="67" t="inlineStr">
+        <is>
+          <t>HS-034</t>
+        </is>
+      </c>
+      <c r="B25" s="73" t="inlineStr">
+        <is>
+          <t>HS-033</t>
+        </is>
+      </c>
+      <c r="C25" s="68" t="n">
+        <v>208.107</v>
+      </c>
+      <c r="D25" s="68" t="n">
+        <v>207.8</v>
+      </c>
+      <c r="E25" s="68" t="n">
+        <v>205.487</v>
+      </c>
+      <c r="F25" s="69" t="n">
+        <v>205.3</v>
+      </c>
+      <c r="G25" s="68" t="n">
+        <v>55.29</v>
+      </c>
       <c r="H25" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -2986,7 +3429,9 @@
         <f>J25+M25+0.1</f>
         <v/>
       </c>
-      <c r="L25" s="73" t="n"/>
+      <c r="L25" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M25" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -3021,15 +3466,38 @@
         <f>2*G25*(K25-O25+0.05)</f>
         <v/>
       </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="14.65" customHeight="1" s="45">
-      <c r="A26" s="67" t="n"/>
-      <c r="B26" s="73" t="n"/>
-      <c r="C26" s="68" t="n"/>
-      <c r="D26" s="68" t="n"/>
-      <c r="E26" s="68" t="n"/>
-      <c r="F26" s="69" t="n"/>
-      <c r="G26" s="68" t="n"/>
+      <c r="A26" s="67" t="inlineStr">
+        <is>
+          <t>HS-035</t>
+        </is>
+      </c>
+      <c r="B26" s="73" t="inlineStr">
+        <is>
+          <t>HS-034</t>
+        </is>
+      </c>
+      <c r="C26" s="68" t="n">
+        <v>208.7</v>
+      </c>
+      <c r="D26" s="68" t="n">
+        <v>208.107</v>
+      </c>
+      <c r="E26" s="68" t="n">
+        <v>205.64</v>
+      </c>
+      <c r="F26" s="69" t="n">
+        <v>205.487</v>
+      </c>
+      <c r="G26" s="68" t="n">
+        <v>55.12</v>
+      </c>
       <c r="H26" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -3045,7 +3513,9 @@
         <f>J26+M26+0.1</f>
         <v/>
       </c>
-      <c r="L26" s="73" t="n"/>
+      <c r="L26" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M26" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -3080,15 +3550,38 @@
         <f>2*G26*(K26-O26+0.05)</f>
         <v/>
       </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="14.65" customHeight="1" s="45">
-      <c r="A27" s="67" t="n"/>
-      <c r="B27" s="73" t="n"/>
-      <c r="C27" s="68" t="n"/>
-      <c r="D27" s="68" t="n"/>
-      <c r="E27" s="68" t="n"/>
-      <c r="F27" s="69" t="n"/>
-      <c r="G27" s="68" t="n"/>
+      <c r="A27" s="67" t="inlineStr">
+        <is>
+          <t>HS-036</t>
+        </is>
+      </c>
+      <c r="B27" s="73" t="inlineStr">
+        <is>
+          <t>HS-035</t>
+        </is>
+      </c>
+      <c r="C27" s="68" t="n">
+        <v>208.27</v>
+      </c>
+      <c r="D27" s="68" t="n">
+        <v>208.7</v>
+      </c>
+      <c r="E27" s="68" t="n">
+        <v>205.77</v>
+      </c>
+      <c r="F27" s="69" t="n">
+        <v>205.64</v>
+      </c>
+      <c r="G27" s="68" t="n">
+        <v>55.34</v>
+      </c>
       <c r="H27" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -3104,7 +3597,9 @@
         <f>J27+M27+0.1</f>
         <v/>
       </c>
-      <c r="L27" s="73" t="n"/>
+      <c r="L27" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M27" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -3139,15 +3634,38 @@
         <f>2*G27*(K27-O27+0.05)</f>
         <v/>
       </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="14.65" customHeight="1" s="45">
-      <c r="A28" s="67" t="n"/>
-      <c r="B28" s="73" t="n"/>
-      <c r="C28" s="68" t="n"/>
-      <c r="D28" s="68" t="n"/>
-      <c r="E28" s="68" t="n"/>
-      <c r="F28" s="69" t="n"/>
-      <c r="G28" s="68" t="n"/>
+      <c r="A28" s="67" t="inlineStr">
+        <is>
+          <t>HS-037</t>
+        </is>
+      </c>
+      <c r="B28" s="73" t="inlineStr">
+        <is>
+          <t>HS-036</t>
+        </is>
+      </c>
+      <c r="C28" s="68" t="n">
+        <v>209.29</v>
+      </c>
+      <c r="D28" s="68" t="n">
+        <v>208.27</v>
+      </c>
+      <c r="E28" s="68" t="n">
+        <v>205.79</v>
+      </c>
+      <c r="F28" s="69" t="n">
+        <v>205.77</v>
+      </c>
+      <c r="G28" s="68" t="n">
+        <v>54</v>
+      </c>
       <c r="H28" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -3163,7 +3681,9 @@
         <f>J28+M28+0.1</f>
         <v/>
       </c>
-      <c r="L28" s="73" t="n"/>
+      <c r="L28" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M28" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -3198,15 +3718,38 @@
         <f>2*G28*(K28-O28+0.05)</f>
         <v/>
       </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="14.65" customHeight="1" s="45">
-      <c r="A29" s="67" t="n"/>
-      <c r="B29" s="73" t="n"/>
-      <c r="C29" s="68" t="n"/>
-      <c r="D29" s="68" t="n"/>
-      <c r="E29" s="68" t="n"/>
-      <c r="F29" s="69" t="n"/>
-      <c r="G29" s="68" t="n"/>
+      <c r="A29" s="67" t="inlineStr">
+        <is>
+          <t>HS-039</t>
+        </is>
+      </c>
+      <c r="B29" s="73" t="inlineStr">
+        <is>
+          <t>HS-038</t>
+        </is>
+      </c>
+      <c r="C29" s="68" t="n">
+        <v>208.82</v>
+      </c>
+      <c r="D29" s="68" t="n">
+        <v>208.54</v>
+      </c>
+      <c r="E29" s="68" t="n">
+        <v>206.12</v>
+      </c>
+      <c r="F29" s="69" t="n">
+        <v>205.99</v>
+      </c>
+      <c r="G29" s="68" t="n">
+        <v>50.05</v>
+      </c>
       <c r="H29" s="70" t="n">
         <v>1.2</v>
       </c>
@@ -3222,7 +3765,9 @@
         <f>J29+M29+0.1</f>
         <v/>
       </c>
-      <c r="L29" s="73" t="n"/>
+      <c r="L29" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M29" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -3257,15 +3802,38 @@
         <f>2*G29*(K29-O29+0.05)</f>
         <v/>
       </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="14.65" customHeight="1" s="45">
-      <c r="A30" s="76" t="n"/>
-      <c r="B30" s="73" t="n"/>
-      <c r="C30" s="68" t="n"/>
-      <c r="D30" s="68" t="n"/>
-      <c r="E30" s="68" t="n"/>
-      <c r="F30" s="69" t="n"/>
-      <c r="G30" s="82" t="n"/>
+      <c r="A30" s="76" t="inlineStr">
+        <is>
+          <t>HS-038</t>
+        </is>
+      </c>
+      <c r="B30" s="73" t="inlineStr">
+        <is>
+          <t>HS-037</t>
+        </is>
+      </c>
+      <c r="C30" s="68" t="n">
+        <v>208.54</v>
+      </c>
+      <c r="D30" s="68" t="n">
+        <v>209.29</v>
+      </c>
+      <c r="E30" s="68" t="n">
+        <v>205.99</v>
+      </c>
+      <c r="F30" s="69" t="n">
+        <v>205.79</v>
+      </c>
+      <c r="G30" s="82" t="n">
+        <v>51.46</v>
+      </c>
       <c r="H30" s="78" t="n">
         <v>1.1</v>
       </c>
@@ -3281,7 +3849,9 @@
         <f>J30+M30+0.1</f>
         <v/>
       </c>
-      <c r="L30" s="81" t="n"/>
+      <c r="L30" s="81" t="n">
+        <v>480</v>
+      </c>
       <c r="M30" s="74" t="n">
         <v>0.04</v>
       </c>
@@ -3316,20 +3886,45 @@
         <f>2*G30*(K30-O30+0.05)</f>
         <v/>
       </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="14.65" customHeight="1" s="45">
-      <c r="A31" s="67" t="n"/>
-      <c r="B31" s="73" t="n"/>
-      <c r="C31" s="68" t="n"/>
-      <c r="D31" s="68" t="n"/>
-      <c r="E31" s="68" t="n"/>
-      <c r="F31" s="69" t="n"/>
-      <c r="G31" s="83" t="n"/>
+      <c r="A31" s="67" t="inlineStr">
+        <is>
+          <t>HS-040</t>
+        </is>
+      </c>
+      <c r="B31" s="73" t="inlineStr">
+        <is>
+          <t>HS-039</t>
+        </is>
+      </c>
+      <c r="C31" s="68" t="n">
+        <v>209.2</v>
+      </c>
+      <c r="D31" s="68" t="n">
+        <v>208.82</v>
+      </c>
+      <c r="E31" s="68" t="n">
+        <v>206.7</v>
+      </c>
+      <c r="F31" s="69" t="n">
+        <v>206.12</v>
+      </c>
+      <c r="G31" s="83" t="n">
+        <v>42.79</v>
+      </c>
       <c r="H31" s="71" t="n"/>
       <c r="I31" s="71" t="n"/>
       <c r="J31" s="71" t="n"/>
       <c r="K31" s="72" t="n"/>
-      <c r="L31" s="73" t="n"/>
+      <c r="L31" s="73" t="n">
+        <v>480</v>
+      </c>
       <c r="M31" s="58" t="n"/>
       <c r="N31" s="72" t="n"/>
       <c r="O31" s="71" t="n"/>
@@ -3339,20 +3934,45 @@
       <c r="S31" s="71" t="n"/>
       <c r="T31" s="71" t="n"/>
       <c r="U31" s="75" t="n"/>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="14.65" customHeight="1" s="45">
-      <c r="A32" s="84" t="n"/>
-      <c r="B32" s="85" t="n"/>
-      <c r="C32" s="86" t="n"/>
-      <c r="D32" s="86" t="n"/>
-      <c r="E32" s="86" t="n"/>
-      <c r="F32" s="87" t="n"/>
-      <c r="G32" s="86" t="n"/>
+      <c r="A32" s="84" t="inlineStr">
+        <is>
+          <t>H-025</t>
+        </is>
+      </c>
+      <c r="B32" s="85" t="inlineStr">
+        <is>
+          <t>24_Rï¿½</t>
+        </is>
+      </c>
+      <c r="C32" s="86" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="D32" s="86" t="n">
+        <v>207.34</v>
+      </c>
+      <c r="E32" s="86" t="n">
+        <v>203.37</v>
+      </c>
+      <c r="F32" s="87" t="n">
+        <v>203.3</v>
+      </c>
+      <c r="G32" s="86" t="n">
+        <v>20.7</v>
+      </c>
       <c r="H32" s="88" t="n"/>
       <c r="I32" s="88" t="n"/>
       <c r="J32" s="88" t="n"/>
       <c r="K32" s="89" t="n"/>
-      <c r="L32" s="85" t="n"/>
+      <c r="L32" s="85" t="n">
+        <v>800</v>
+      </c>
       <c r="M32" s="90" t="n"/>
       <c r="N32" s="89" t="n"/>
       <c r="O32" s="88" t="n"/>
@@ -3362,15 +3982,3413 @@
       <c r="S32" s="88" t="n"/>
       <c r="T32" s="88" t="n"/>
       <c r="U32" s="91" t="n"/>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="14.65" customHeight="1" s="45">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>H-025.2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>H-025</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>206.85</v>
+      </c>
+      <c r="D33" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="E33" t="n">
+        <v>204.17</v>
+      </c>
+      <c r="F33" t="n">
+        <v>203.37</v>
+      </c>
+      <c r="G33" t="n">
+        <v>21.57</v>
+      </c>
       <c r="I33" s="92" t="n"/>
+      <c r="L33" t="n">
+        <v>500</v>
+      </c>
       <c r="P33" s="93" t="n"/>
       <c r="Q33" s="93" t="n"/>
       <c r="R33" s="93" t="n"/>
       <c r="S33" s="93" t="n"/>
       <c r="T33" s="93" t="n"/>
       <c r="U33" s="93" t="n"/>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>HS-027</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>H-026</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="D34" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="E34" t="n">
+        <v>204.59</v>
+      </c>
+      <c r="F34" t="n">
+        <v>203.76</v>
+      </c>
+      <c r="G34" t="n">
+        <v>52.42</v>
+      </c>
+      <c r="L34" t="n">
+        <v>500</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>H-026</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>H-025</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="D35" t="n">
+        <v>206.83</v>
+      </c>
+      <c r="E35" t="n">
+        <v>203.76</v>
+      </c>
+      <c r="F35" t="n">
+        <v>203.37</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4</v>
+      </c>
+      <c r="L35" t="n">
+        <v>600</v>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>M3540</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>M3541</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>227.74</v>
+      </c>
+      <c r="D36" t="n">
+        <v>224.23</v>
+      </c>
+      <c r="E36" t="n">
+        <v>225.6</v>
+      </c>
+      <c r="F36" t="n">
+        <v>222.13</v>
+      </c>
+      <c r="G36" t="n">
+        <v>49.12</v>
+      </c>
+      <c r="L36" t="n">
+        <v>315</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>M3541</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>M3542</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>224.23</v>
+      </c>
+      <c r="D37" t="n">
+        <v>221.34</v>
+      </c>
+      <c r="E37" t="n">
+        <v>222.13</v>
+      </c>
+      <c r="F37" t="n">
+        <v>219.32</v>
+      </c>
+      <c r="G37" t="n">
+        <v>49.07</v>
+      </c>
+      <c r="L37" t="n">
+        <v>315</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>M3543</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>M3542</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>219.4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>221.34</v>
+      </c>
+      <c r="E38" t="n">
+        <v>217.3</v>
+      </c>
+      <c r="F38" t="n">
+        <v>219.32</v>
+      </c>
+      <c r="G38" t="n">
+        <v>49.04</v>
+      </c>
+      <c r="L38" t="n">
+        <v>400</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>M3543</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>M3544</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>219.4</v>
+      </c>
+      <c r="D39" t="n">
+        <v>219.01</v>
+      </c>
+      <c r="E39" t="n">
+        <v>217.3</v>
+      </c>
+      <c r="F39" t="n">
+        <v>216.9</v>
+      </c>
+      <c r="G39" t="n">
+        <v>23</v>
+      </c>
+      <c r="L39" t="n">
+        <v>500</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>M3544</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>M3545</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>219.01</v>
+      </c>
+      <c r="D40" t="n">
+        <v>218.93</v>
+      </c>
+      <c r="E40" t="n">
+        <v>216.9</v>
+      </c>
+      <c r="F40" t="n">
+        <v>216.77</v>
+      </c>
+      <c r="G40" t="n">
+        <v>23</v>
+      </c>
+      <c r="L40" t="n">
+        <v>630</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>M3545</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>M3546</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>218.93</v>
+      </c>
+      <c r="D41" t="n">
+        <v>218.82</v>
+      </c>
+      <c r="E41" t="n">
+        <v>216.77</v>
+      </c>
+      <c r="F41" t="n">
+        <v>216.63</v>
+      </c>
+      <c r="G41" t="n">
+        <v>25</v>
+      </c>
+      <c r="L41" t="n">
+        <v>630</v>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>M3546</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>M3547</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>218.82</v>
+      </c>
+      <c r="D42" t="n">
+        <v>217.67</v>
+      </c>
+      <c r="E42" t="n">
+        <v>216.63</v>
+      </c>
+      <c r="F42" t="n">
+        <v>215.55</v>
+      </c>
+      <c r="G42" t="n">
+        <v>61.01</v>
+      </c>
+      <c r="L42" t="n">
+        <v>630</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>M3547</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>M3548</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>217.67</v>
+      </c>
+      <c r="D43" t="n">
+        <v>214.46</v>
+      </c>
+      <c r="E43" t="n">
+        <v>215.55</v>
+      </c>
+      <c r="F43" t="n">
+        <v>212.19</v>
+      </c>
+      <c r="G43" t="n">
+        <v>73.08</v>
+      </c>
+      <c r="L43" t="n">
+        <v>630</v>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>M3548</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>M3549</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>214.46</v>
+      </c>
+      <c r="D44" t="n">
+        <v>213.92</v>
+      </c>
+      <c r="E44" t="n">
+        <v>212.19</v>
+      </c>
+      <c r="F44" t="n">
+        <v>211.91</v>
+      </c>
+      <c r="G44" t="n">
+        <v>27</v>
+      </c>
+      <c r="L44" t="n">
+        <v>630</v>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>M3549</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>M3550</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>213.92</v>
+      </c>
+      <c r="D45" t="n">
+        <v>213.84</v>
+      </c>
+      <c r="E45" t="n">
+        <v>211.91</v>
+      </c>
+      <c r="F45" t="n">
+        <v>211.39</v>
+      </c>
+      <c r="G45" t="n">
+        <v>41</v>
+      </c>
+      <c r="L45" t="n">
+        <v>630</v>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>M3551</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>M3552</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>215.21</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>213.13</v>
+      </c>
+      <c r="F46" t="n">
+        <v>211.63</v>
+      </c>
+      <c r="G46" t="n">
+        <v>65.02</v>
+      </c>
+      <c r="L46" t="n">
+        <v>315</v>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>M3552</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>M3553</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>213.67</v>
+      </c>
+      <c r="E47" t="n">
+        <v>211.63</v>
+      </c>
+      <c r="F47" t="n">
+        <v>211.39</v>
+      </c>
+      <c r="G47" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="L47" t="n">
+        <v>400</v>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>M3553</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>M3554</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>213.67</v>
+      </c>
+      <c r="D48" t="n">
+        <v>213.73</v>
+      </c>
+      <c r="E48" t="n">
+        <v>211.39</v>
+      </c>
+      <c r="F48" t="n">
+        <v>211.12</v>
+      </c>
+      <c r="G48" t="n">
+        <v>33.87</v>
+      </c>
+      <c r="L48" t="n">
+        <v>400</v>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>M3550</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>M3554</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>213.84</v>
+      </c>
+      <c r="D49" t="n">
+        <v>213.73</v>
+      </c>
+      <c r="E49" t="n">
+        <v>211.39</v>
+      </c>
+      <c r="F49" t="n">
+        <v>211.12</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="L49" t="n">
+        <v>630</v>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>M3555</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>M3556</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>216.5</v>
+      </c>
+      <c r="D50" t="n">
+        <v>215.01</v>
+      </c>
+      <c r="E50" t="n">
+        <v>214.82</v>
+      </c>
+      <c r="F50" t="n">
+        <v>211.9</v>
+      </c>
+      <c r="G50" t="n">
+        <v>6.86</v>
+      </c>
+      <c r="L50" t="n">
+        <v>400</v>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>M3556</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>M3557</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>215.01</v>
+      </c>
+      <c r="D51" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="E51" t="n">
+        <v>211.9</v>
+      </c>
+      <c r="F51" t="n">
+        <v>211.53</v>
+      </c>
+      <c r="G51" t="n">
+        <v>36.85</v>
+      </c>
+      <c r="L51" t="n">
+        <v>500</v>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>M3557</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>M3559</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="D52" t="n">
+        <v>213.48</v>
+      </c>
+      <c r="E52" t="n">
+        <v>211.53</v>
+      </c>
+      <c r="F52" t="n">
+        <v>211.47</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="L52" t="n">
+        <v>500</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>M3558</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>M3559</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>213.1</v>
+      </c>
+      <c r="D53" t="n">
+        <v>213.48</v>
+      </c>
+      <c r="E53" t="n">
+        <v>211.66</v>
+      </c>
+      <c r="F53" t="n">
+        <v>211.47</v>
+      </c>
+      <c r="G53" t="n">
+        <v>11.93</v>
+      </c>
+      <c r="L53" t="n">
+        <v>315</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>M3559</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>N1321</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>213.48</v>
+      </c>
+      <c r="D54" t="n">
+        <v>210.336</v>
+      </c>
+      <c r="E54" t="n">
+        <v>211.47</v>
+      </c>
+      <c r="F54" t="n">
+        <v>208</v>
+      </c>
+      <c r="G54" t="n">
+        <v>28.27</v>
+      </c>
+      <c r="L54" t="n">
+        <v>300</v>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>N1321</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1306</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>210.336</v>
+      </c>
+      <c r="D55" t="n">
+        <v>209.57</v>
+      </c>
+      <c r="E55" t="n">
+        <v>208</v>
+      </c>
+      <c r="F55" t="n">
+        <v>207.17</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="L55" t="n">
+        <v>300</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>N1322</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>N1321</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>209.254</v>
+      </c>
+      <c r="D56" t="n">
+        <v>210.336</v>
+      </c>
+      <c r="E56" t="n">
+        <v>208.25</v>
+      </c>
+      <c r="F56" t="n">
+        <v>208</v>
+      </c>
+      <c r="G56" t="n">
+        <v>44.24</v>
+      </c>
+      <c r="L56" t="n">
+        <v>300</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>N1323</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>N1324</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>207.427</v>
+      </c>
+      <c r="D57" t="n">
+        <v>207.27</v>
+      </c>
+      <c r="E57" t="n">
+        <v>206.85</v>
+      </c>
+      <c r="F57" t="n">
+        <v>206.8</v>
+      </c>
+      <c r="G57" t="n">
+        <v>33.28</v>
+      </c>
+      <c r="L57" t="n">
+        <v>300</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>N1324</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>N1327.1</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>207.27</v>
+      </c>
+      <c r="D58" t="n">
+        <v>207.125</v>
+      </c>
+      <c r="E58" t="n">
+        <v>206.8</v>
+      </c>
+      <c r="F58" t="n">
+        <v>206.58</v>
+      </c>
+      <c r="G58" t="n">
+        <v>47.14</v>
+      </c>
+      <c r="L58" t="n">
+        <v>300</v>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>N1325</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>N1324</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>207.883</v>
+      </c>
+      <c r="D59" t="n">
+        <v>207.27</v>
+      </c>
+      <c r="E59" t="n">
+        <v>207</v>
+      </c>
+      <c r="F59" t="n">
+        <v>206.8</v>
+      </c>
+      <c r="G59" t="n">
+        <v>36.23</v>
+      </c>
+      <c r="L59" t="n">
+        <v>300</v>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>N1325.1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>N1325</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>208.147</v>
+      </c>
+      <c r="D60" t="n">
+        <v>207.883</v>
+      </c>
+      <c r="E60" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="F60" t="n">
+        <v>207</v>
+      </c>
+      <c r="G60" t="n">
+        <v>36.49</v>
+      </c>
+      <c r="L60" t="n">
+        <v>300</v>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>N1327.1</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1327.1</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>207.125</v>
+      </c>
+      <c r="D61" t="n">
+        <v>207.097</v>
+      </c>
+      <c r="E61" t="n">
+        <v>206.58</v>
+      </c>
+      <c r="F61" t="n">
+        <v>206.4</v>
+      </c>
+      <c r="G61" t="n">
+        <v>22.51</v>
+      </c>
+      <c r="L61" t="n">
+        <v>400</v>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>N1331-1</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>N1331-2</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>210.746</v>
+      </c>
+      <c r="D62" t="n">
+        <v>208.812</v>
+      </c>
+      <c r="E62" t="n">
+        <v>207.796</v>
+      </c>
+      <c r="F62" t="n">
+        <v>207.293</v>
+      </c>
+      <c r="G62" t="n">
+        <v>34.71</v>
+      </c>
+      <c r="L62" t="n">
+        <v>400</v>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>N1331-2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>N1331-3</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>208.812</v>
+      </c>
+      <c r="D63" t="n">
+        <v>207.771</v>
+      </c>
+      <c r="E63" t="n">
+        <v>207.293</v>
+      </c>
+      <c r="F63" t="n">
+        <v>206.813</v>
+      </c>
+      <c r="G63" t="n">
+        <v>44.22</v>
+      </c>
+      <c r="L63" t="n">
+        <v>400</v>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>N1331-3</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>N1331-4</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>207.771</v>
+      </c>
+      <c r="D64" t="n">
+        <v>207.629</v>
+      </c>
+      <c r="E64" t="n">
+        <v>206.813</v>
+      </c>
+      <c r="F64" t="n">
+        <v>206.289</v>
+      </c>
+      <c r="G64" t="n">
+        <v>43.84</v>
+      </c>
+      <c r="L64" t="n">
+        <v>400</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>N1331-4</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>N1331-5</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>207.629</v>
+      </c>
+      <c r="D65" t="n">
+        <v>207.183</v>
+      </c>
+      <c r="E65" t="n">
+        <v>206.289</v>
+      </c>
+      <c r="F65" t="n">
+        <v>205.8</v>
+      </c>
+      <c r="G65" t="n">
+        <v>48.17</v>
+      </c>
+      <c r="L65" t="n">
+        <v>400</v>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>N1331-5</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>N1331-6</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>207.183</v>
+      </c>
+      <c r="D66" t="n">
+        <v>207.034</v>
+      </c>
+      <c r="E66" t="n">
+        <v>205.8</v>
+      </c>
+      <c r="F66" t="n">
+        <v>205.358</v>
+      </c>
+      <c r="G66" t="n">
+        <v>29.11</v>
+      </c>
+      <c r="L66" t="n">
+        <v>600</v>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>N1331-6</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>W_Rï¿½</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>207.034</v>
+      </c>
+      <c r="D67" t="n">
+        <v>208.514</v>
+      </c>
+      <c r="E67" t="n">
+        <v>205.358</v>
+      </c>
+      <c r="F67" t="n">
+        <v>204.4</v>
+      </c>
+      <c r="G67" t="n">
+        <v>38.95</v>
+      </c>
+      <c r="L67" t="n">
+        <v>600</v>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>N1332</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>N1331-1</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>210.477</v>
+      </c>
+      <c r="D68" t="n">
+        <v>210.746</v>
+      </c>
+      <c r="E68" t="n">
+        <v>208.502</v>
+      </c>
+      <c r="F68" t="n">
+        <v>207.796</v>
+      </c>
+      <c r="G68" t="n">
+        <v>62.47</v>
+      </c>
+      <c r="L68" t="n">
+        <v>400</v>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>N1333</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>N1332</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>211.22</v>
+      </c>
+      <c r="D69" t="n">
+        <v>210.477</v>
+      </c>
+      <c r="E69" t="n">
+        <v>209.69</v>
+      </c>
+      <c r="F69" t="n">
+        <v>208.502</v>
+      </c>
+      <c r="G69" t="n">
+        <v>64.81</v>
+      </c>
+      <c r="L69" t="n">
+        <v>400</v>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>N1334</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>N1333</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>214.681</v>
+      </c>
+      <c r="D70" t="n">
+        <v>211.22</v>
+      </c>
+      <c r="E70" t="n">
+        <v>212.413</v>
+      </c>
+      <c r="F70" t="n">
+        <v>209.69</v>
+      </c>
+      <c r="G70" t="n">
+        <v>77.67</v>
+      </c>
+      <c r="L70" t="n">
+        <v>400</v>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>N1337</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>N1334</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>219.273</v>
+      </c>
+      <c r="D71" t="n">
+        <v>214.681</v>
+      </c>
+      <c r="E71" t="n">
+        <v>216</v>
+      </c>
+      <c r="F71" t="n">
+        <v>212.413</v>
+      </c>
+      <c r="G71" t="n">
+        <v>43.27</v>
+      </c>
+      <c r="L71" t="n">
+        <v>400</v>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>1288</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>765</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>212.45</v>
+      </c>
+      <c r="D72" t="n">
+        <v>211.3</v>
+      </c>
+      <c r="E72" t="n">
+        <v>210.4</v>
+      </c>
+      <c r="F72" t="n">
+        <v>208.79</v>
+      </c>
+      <c r="G72" t="n">
+        <v>60.32</v>
+      </c>
+      <c r="L72" t="n">
+        <v>500</v>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>1289</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1288</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>212.75</v>
+      </c>
+      <c r="D73" t="n">
+        <v>212.45</v>
+      </c>
+      <c r="E73" t="n">
+        <v>210.98</v>
+      </c>
+      <c r="F73" t="n">
+        <v>210.4</v>
+      </c>
+      <c r="G73" t="n">
+        <v>35.08</v>
+      </c>
+      <c r="L73" t="n">
+        <v>300</v>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>1306</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1307</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>209.57</v>
+      </c>
+      <c r="D74" t="n">
+        <v>207.309</v>
+      </c>
+      <c r="E74" t="n">
+        <v>207.17</v>
+      </c>
+      <c r="F74" t="n">
+        <v>206.17</v>
+      </c>
+      <c r="G74" t="n">
+        <v>68.48999999999999</v>
+      </c>
+      <c r="L74" t="n">
+        <v>500</v>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>1307</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>H-025.2</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>207.309</v>
+      </c>
+      <c r="D75" t="n">
+        <v>206.85</v>
+      </c>
+      <c r="E75" t="n">
+        <v>206.17</v>
+      </c>
+      <c r="F75" t="n">
+        <v>204.17</v>
+      </c>
+      <c r="G75" t="n">
+        <v>45.97</v>
+      </c>
+      <c r="L75" t="n">
+        <v>500</v>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>1321</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1322</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>210.82</v>
+      </c>
+      <c r="D76" t="n">
+        <v>210.25</v>
+      </c>
+      <c r="E76" t="n">
+        <v>209.24</v>
+      </c>
+      <c r="F76" t="n">
+        <v>208.4</v>
+      </c>
+      <c r="G76" t="n">
+        <v>43.36</v>
+      </c>
+      <c r="L76" t="n">
+        <v>250</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>1322</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1323</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>210.25</v>
+      </c>
+      <c r="D77" t="n">
+        <v>209.49</v>
+      </c>
+      <c r="E77" t="n">
+        <v>208.4</v>
+      </c>
+      <c r="F77" t="n">
+        <v>207.58</v>
+      </c>
+      <c r="G77" t="n">
+        <v>41.96</v>
+      </c>
+      <c r="L77" t="n">
+        <v>250</v>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>1323</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1324</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>209.49</v>
+      </c>
+      <c r="D78" t="n">
+        <v>208.56</v>
+      </c>
+      <c r="E78" t="n">
+        <v>207.58</v>
+      </c>
+      <c r="F78" t="n">
+        <v>207.05</v>
+      </c>
+      <c r="G78" t="n">
+        <v>50.62</v>
+      </c>
+      <c r="L78" t="n">
+        <v>300</v>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>1324</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1326</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>208.56</v>
+      </c>
+      <c r="D79" t="n">
+        <v>207.59</v>
+      </c>
+      <c r="E79" t="n">
+        <v>207.05</v>
+      </c>
+      <c r="F79" t="n">
+        <v>206.81</v>
+      </c>
+      <c r="G79" t="n">
+        <v>28.01</v>
+      </c>
+      <c r="L79" t="n">
+        <v>300</v>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>1325</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1324</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>209.84</v>
+      </c>
+      <c r="D80" t="n">
+        <v>208.56</v>
+      </c>
+      <c r="E80" t="n">
+        <v>208.43</v>
+      </c>
+      <c r="F80" t="n">
+        <v>207.05</v>
+      </c>
+      <c r="G80" t="n">
+        <v>28.99</v>
+      </c>
+      <c r="L80" t="n">
+        <v>250</v>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>1325.1</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1325</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>210.5</v>
+      </c>
+      <c r="D81" t="n">
+        <v>209.84</v>
+      </c>
+      <c r="E81" t="n">
+        <v>209.5</v>
+      </c>
+      <c r="F81" t="n">
+        <v>208.43</v>
+      </c>
+      <c r="G81" t="n">
+        <v>22.03</v>
+      </c>
+      <c r="L81" t="n">
+        <v>250</v>
+      </c>
+      <c r="W81" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>1326</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1327</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>207.59</v>
+      </c>
+      <c r="D82" t="n">
+        <v>207.25</v>
+      </c>
+      <c r="E82" t="n">
+        <v>206.81</v>
+      </c>
+      <c r="F82" t="n">
+        <v>206.63</v>
+      </c>
+      <c r="G82" t="n">
+        <v>38.39</v>
+      </c>
+      <c r="L82" t="n">
+        <v>300</v>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>1327</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>N1327.1</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>207.25</v>
+      </c>
+      <c r="D83" t="n">
+        <v>207.125</v>
+      </c>
+      <c r="E83" t="n">
+        <v>206.63</v>
+      </c>
+      <c r="F83" t="n">
+        <v>206.58</v>
+      </c>
+      <c r="G83" t="n">
+        <v>18.99</v>
+      </c>
+      <c r="L83" t="n">
+        <v>400</v>
+      </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>1327.1</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1307</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>207.097</v>
+      </c>
+      <c r="D84" t="n">
+        <v>207.309</v>
+      </c>
+      <c r="E84" t="n">
+        <v>206.4</v>
+      </c>
+      <c r="F84" t="n">
+        <v>206.17</v>
+      </c>
+      <c r="G84" t="n">
+        <v>34.37</v>
+      </c>
+      <c r="L84" t="n">
+        <v>400</v>
+      </c>
+      <c r="W84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>1330</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1329</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>211.73</v>
+      </c>
+      <c r="D85" t="n">
+        <v>209.16</v>
+      </c>
+      <c r="E85" t="n">
+        <v>209.77</v>
+      </c>
+      <c r="F85" t="n">
+        <v>208.16</v>
+      </c>
+      <c r="G85" t="n">
+        <v>43.45</v>
+      </c>
+      <c r="L85" t="n">
+        <v>300</v>
+      </c>
+      <c r="W85" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>1331</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1330</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>213.95</v>
+      </c>
+      <c r="D86" t="n">
+        <v>211.73</v>
+      </c>
+      <c r="E86" t="n">
+        <v>212.51</v>
+      </c>
+      <c r="F86" t="n">
+        <v>209.77</v>
+      </c>
+      <c r="G86" t="n">
+        <v>44.92</v>
+      </c>
+      <c r="L86" t="n">
+        <v>300</v>
+      </c>
+      <c r="W86" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>1332</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1331</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>217.26</v>
+      </c>
+      <c r="D87" t="n">
+        <v>213.95</v>
+      </c>
+      <c r="E87" t="n">
+        <v>216.02</v>
+      </c>
+      <c r="F87" t="n">
+        <v>212.51</v>
+      </c>
+      <c r="G87" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="L87" t="n">
+        <v>300</v>
+      </c>
+      <c r="W87" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>1333</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1332</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>216.2</v>
+      </c>
+      <c r="D88" t="n">
+        <v>217.26</v>
+      </c>
+      <c r="E88" t="n">
+        <v>214.74</v>
+      </c>
+      <c r="F88" t="n">
+        <v>216.02</v>
+      </c>
+      <c r="G88" t="n">
+        <v>51.45</v>
+      </c>
+      <c r="L88" t="n">
+        <v>300</v>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>1334</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1333</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>216</v>
+      </c>
+      <c r="D89" t="n">
+        <v>216.2</v>
+      </c>
+      <c r="E89" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="F89" t="n">
+        <v>214.74</v>
+      </c>
+      <c r="G89" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="L89" t="n">
+        <v>300</v>
+      </c>
+      <c r="W89" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>1335</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1334</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>218.09</v>
+      </c>
+      <c r="D90" t="n">
+        <v>216</v>
+      </c>
+      <c r="E90" t="n">
+        <v>216.54</v>
+      </c>
+      <c r="F90" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G90" t="n">
+        <v>43.24</v>
+      </c>
+      <c r="L90" t="n">
+        <v>300</v>
+      </c>
+      <c r="W90" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>1336</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>1335</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>219.72</v>
+      </c>
+      <c r="D91" t="n">
+        <v>218.09</v>
+      </c>
+      <c r="E91" t="n">
+        <v>218.17</v>
+      </c>
+      <c r="F91" t="n">
+        <v>216.54</v>
+      </c>
+      <c r="G91" t="n">
+        <v>32.85</v>
+      </c>
+      <c r="L91" t="n">
+        <v>300</v>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>1337</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1336</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>222.51</v>
+      </c>
+      <c r="D92" t="n">
+        <v>219.72</v>
+      </c>
+      <c r="E92" t="n">
+        <v>220.36</v>
+      </c>
+      <c r="F92" t="n">
+        <v>218.17</v>
+      </c>
+      <c r="G92" t="n">
+        <v>33.15</v>
+      </c>
+      <c r="L92" t="n">
+        <v>300</v>
+      </c>
+      <c r="W92" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>1338</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1337</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>225.23</v>
+      </c>
+      <c r="D93" t="n">
+        <v>222.51</v>
+      </c>
+      <c r="E93" t="n">
+        <v>223.31</v>
+      </c>
+      <c r="F93" t="n">
+        <v>220.36</v>
+      </c>
+      <c r="G93" t="n">
+        <v>46.28</v>
+      </c>
+      <c r="L93" t="n">
+        <v>300</v>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>1341</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>HS-037</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>209.25</v>
+      </c>
+      <c r="D94" t="n">
+        <v>209.29</v>
+      </c>
+      <c r="E94" t="n">
+        <v>207.87</v>
+      </c>
+      <c r="F94" t="n">
+        <v>205.79</v>
+      </c>
+      <c r="G94" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="L94" t="n">
+        <v>200</v>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>1342RU</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1341</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>209.86</v>
+      </c>
+      <c r="D95" t="n">
+        <v>209.25</v>
+      </c>
+      <c r="E95" t="n">
+        <v>207.65</v>
+      </c>
+      <c r="F95" t="n">
+        <v>207.87</v>
+      </c>
+      <c r="G95" t="n">
+        <v>32.01</v>
+      </c>
+      <c r="L95" t="n">
+        <v>200</v>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>1342RU</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1342.0AL</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>209.86</v>
+      </c>
+      <c r="D96" t="n">
+        <v>205.6</v>
+      </c>
+      <c r="E96" t="n">
+        <v>207.65</v>
+      </c>
+      <c r="F96" t="n">
+        <v>203.57</v>
+      </c>
+      <c r="G96" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="L96" t="n">
+        <v>500</v>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>1343</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>1342RU</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>212.1</v>
+      </c>
+      <c r="D97" t="n">
+        <v>209.86</v>
+      </c>
+      <c r="E97" t="n">
+        <v>208.37</v>
+      </c>
+      <c r="F97" t="n">
+        <v>207.65</v>
+      </c>
+      <c r="G97" t="n">
+        <v>9.77</v>
+      </c>
+      <c r="L97" t="n">
+        <v>300</v>
+      </c>
+      <c r="W97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>1344</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>1342RU</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>212.19</v>
+      </c>
+      <c r="D98" t="n">
+        <v>209.86</v>
+      </c>
+      <c r="E98" t="n">
+        <v>208.77</v>
+      </c>
+      <c r="F98" t="n">
+        <v>207.65</v>
+      </c>
+      <c r="G98" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="L98" t="n">
+        <v>300</v>
+      </c>
+      <c r="W98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>1345</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>1344</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>215.91</v>
+      </c>
+      <c r="D99" t="n">
+        <v>212.19</v>
+      </c>
+      <c r="E99" t="n">
+        <v>211.31</v>
+      </c>
+      <c r="F99" t="n">
+        <v>208.77</v>
+      </c>
+      <c r="G99" t="n">
+        <v>24.36</v>
+      </c>
+      <c r="L99" t="n">
+        <v>300</v>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>1346</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>1345</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>215.93</v>
+      </c>
+      <c r="D100" t="n">
+        <v>215.91</v>
+      </c>
+      <c r="E100" t="n">
+        <v>214.05</v>
+      </c>
+      <c r="F100" t="n">
+        <v>211.31</v>
+      </c>
+      <c r="G100" t="n">
+        <v>25.27</v>
+      </c>
+      <c r="L100" t="n">
+        <v>300</v>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>1347</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>1346</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>215.96</v>
+      </c>
+      <c r="D101" t="n">
+        <v>215.93</v>
+      </c>
+      <c r="E101" t="n">
+        <v>214.49</v>
+      </c>
+      <c r="F101" t="n">
+        <v>214.05</v>
+      </c>
+      <c r="G101" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="L101" t="n">
+        <v>300</v>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>1348</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1347</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>219.04</v>
+      </c>
+      <c r="D102" t="n">
+        <v>215.96</v>
+      </c>
+      <c r="E102" t="n">
+        <v>215.55</v>
+      </c>
+      <c r="F102" t="n">
+        <v>214.49</v>
+      </c>
+      <c r="G102" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="L102" t="n">
+        <v>300</v>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>1348.1</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1348</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>223.69</v>
+      </c>
+      <c r="D103" t="n">
+        <v>219.04</v>
+      </c>
+      <c r="E103" t="n">
+        <v>220.95</v>
+      </c>
+      <c r="F103" t="n">
+        <v>215.55</v>
+      </c>
+      <c r="G103" t="n">
+        <v>49.76</v>
+      </c>
+      <c r="L103" t="n">
+        <v>300</v>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>1348.2</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>1348.1</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>225.64</v>
+      </c>
+      <c r="D104" t="n">
+        <v>223.69</v>
+      </c>
+      <c r="E104" t="n">
+        <v>223.98</v>
+      </c>
+      <c r="F104" t="n">
+        <v>220.95</v>
+      </c>
+      <c r="G104" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="L104" t="n">
+        <v>300</v>
+      </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>1348.2</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>N1337</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>225.64</v>
+      </c>
+      <c r="D105" t="n">
+        <v>219.273</v>
+      </c>
+      <c r="E105" t="n">
+        <v>223.98</v>
+      </c>
+      <c r="F105" t="n">
+        <v>216</v>
+      </c>
+      <c r="G105" t="n">
+        <v>73.73999999999999</v>
+      </c>
+      <c r="L105" t="n">
+        <v>400</v>
+      </c>
+      <c r="W105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>1349</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>1348.2</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>228.11</v>
+      </c>
+      <c r="D106" t="n">
+        <v>225.64</v>
+      </c>
+      <c r="E106" t="n">
+        <v>225.8</v>
+      </c>
+      <c r="F106" t="n">
+        <v>223.98</v>
+      </c>
+      <c r="G106" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="L106" t="n">
+        <v>400</v>
+      </c>
+      <c r="W106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>1350</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>1349</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>229.22</v>
+      </c>
+      <c r="D107" t="n">
+        <v>228.11</v>
+      </c>
+      <c r="E107" t="n">
+        <v>226.62</v>
+      </c>
+      <c r="F107" t="n">
+        <v>225.8</v>
+      </c>
+      <c r="G107" t="n">
+        <v>31.91</v>
+      </c>
+      <c r="L107" t="n">
+        <v>400</v>
+      </c>
+      <c r="W107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>207.34</v>
+      </c>
+      <c r="D108" t="n">
+        <v>207.61</v>
+      </c>
+      <c r="E108" t="n">
+        <v>203.28</v>
+      </c>
+      <c r="F108" t="n">
+        <v>202.96</v>
+      </c>
+      <c r="G108" t="n">
+        <v>49.85</v>
+      </c>
+      <c r="L108" t="n">
+        <v>800</v>
+      </c>
+      <c r="W108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>24_Rï¿½</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>207.34</v>
+      </c>
+      <c r="D109" t="n">
+        <v>207.34</v>
+      </c>
+      <c r="E109" t="n">
+        <v>203.3</v>
+      </c>
+      <c r="F109" t="n">
+        <v>203.28</v>
+      </c>
+      <c r="G109" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="L109" t="n">
+        <v>800</v>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>744</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Auslauf1</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>208.77</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>205.4</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>209</v>
+      </c>
+      <c r="L110" t="n">
+        <v>500</v>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>745</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>744</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>209.11</v>
+      </c>
+      <c r="D111" t="n">
+        <v>208.77</v>
+      </c>
+      <c r="E111" t="n">
+        <v>205.66</v>
+      </c>
+      <c r="F111" t="n">
+        <v>205.4</v>
+      </c>
+      <c r="G111" t="n">
+        <v>13.29</v>
+      </c>
+      <c r="L111" t="n">
+        <v>300</v>
+      </c>
+      <c r="W111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>746</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>745</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>209.55</v>
+      </c>
+      <c r="D112" t="n">
+        <v>209.11</v>
+      </c>
+      <c r="E112" t="n">
+        <v>205.76</v>
+      </c>
+      <c r="F112" t="n">
+        <v>205.66</v>
+      </c>
+      <c r="G112" t="n">
+        <v>24.94</v>
+      </c>
+      <c r="L112" t="n">
+        <v>300</v>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>747.1</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>747</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>208.38</v>
+      </c>
+      <c r="D113" t="n">
+        <v>207.92</v>
+      </c>
+      <c r="E113" t="n">
+        <v>206.1</v>
+      </c>
+      <c r="F113" t="n">
+        <v>205.93</v>
+      </c>
+      <c r="G113" t="n">
+        <v>46.58</v>
+      </c>
+      <c r="L113" t="n">
+        <v>300</v>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>748</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>747</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>207.95</v>
+      </c>
+      <c r="D114" t="n">
+        <v>207.92</v>
+      </c>
+      <c r="E114" t="n">
+        <v>206.59</v>
+      </c>
+      <c r="F114" t="n">
+        <v>205.93</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="L114" t="n">
+        <v>300</v>
+      </c>
+      <c r="W114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>747</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>746</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>207.92</v>
+      </c>
+      <c r="D115" t="n">
+        <v>209.55</v>
+      </c>
+      <c r="E115" t="n">
+        <v>205.93</v>
+      </c>
+      <c r="F115" t="n">
+        <v>205.76</v>
+      </c>
+      <c r="G115" t="n">
+        <v>62.01</v>
+      </c>
+      <c r="L115" t="n">
+        <v>300</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>747.2</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>747.1</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>207.18</v>
+      </c>
+      <c r="D116" t="n">
+        <v>208.38</v>
+      </c>
+      <c r="E116" t="n">
+        <v>206.17</v>
+      </c>
+      <c r="F116" t="n">
+        <v>206.1</v>
+      </c>
+      <c r="G116" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="L116" t="n">
+        <v>300</v>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>749</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>748</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>209.54</v>
+      </c>
+      <c r="D117" t="n">
+        <v>207.95</v>
+      </c>
+      <c r="E117" t="n">
+        <v>207.74</v>
+      </c>
+      <c r="F117" t="n">
+        <v>206.59</v>
+      </c>
+      <c r="G117" t="n">
+        <v>65.44</v>
+      </c>
+      <c r="L117" t="n">
+        <v>300</v>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>749</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>762</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>209.54</v>
+      </c>
+      <c r="D118" t="n">
+        <v>209.21</v>
+      </c>
+      <c r="E118" t="n">
+        <v>207.74</v>
+      </c>
+      <c r="F118" t="n">
+        <v>206.63</v>
+      </c>
+      <c r="G118" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="L118" t="n">
+        <v>300</v>
+      </c>
+      <c r="W118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>762RU</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>744</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>209.35</v>
+      </c>
+      <c r="D119" t="n">
+        <v>208.77</v>
+      </c>
+      <c r="E119" t="n">
+        <v>206.79</v>
+      </c>
+      <c r="F119" t="n">
+        <v>205.4</v>
+      </c>
+      <c r="G119" t="n">
+        <v>19.25</v>
+      </c>
+      <c r="L119" t="n">
+        <v>400</v>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>762RU</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>762</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>209.35</v>
+      </c>
+      <c r="D120" t="n">
+        <v>209.21</v>
+      </c>
+      <c r="E120" t="n">
+        <v>206.79</v>
+      </c>
+      <c r="F120" t="n">
+        <v>206.63</v>
+      </c>
+      <c r="G120" t="n">
+        <v>18.57</v>
+      </c>
+      <c r="L120" t="n">
+        <v>900</v>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>763</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>762RU</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>209.66</v>
+      </c>
+      <c r="D121" t="n">
+        <v>209.35</v>
+      </c>
+      <c r="E121" t="n">
+        <v>207.54</v>
+      </c>
+      <c r="F121" t="n">
+        <v>206.79</v>
+      </c>
+      <c r="G121" t="n">
+        <v>14.21</v>
+      </c>
+      <c r="L121" t="n">
+        <v>1000</v>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>764</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>763</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>210.06</v>
+      </c>
+      <c r="D122" t="n">
+        <v>209.66</v>
+      </c>
+      <c r="E122" t="n">
+        <v>207.91</v>
+      </c>
+      <c r="F122" t="n">
+        <v>207.54</v>
+      </c>
+      <c r="G122" t="n">
+        <v>18.23</v>
+      </c>
+      <c r="L122" t="n">
+        <v>700</v>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>765</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>764</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>211.3</v>
+      </c>
+      <c r="D123" t="n">
+        <v>210.06</v>
+      </c>
+      <c r="E123" t="n">
+        <v>208.79</v>
+      </c>
+      <c r="F123" t="n">
+        <v>207.91</v>
+      </c>
+      <c r="G123" t="n">
+        <v>47.57</v>
+      </c>
+      <c r="L123" t="n">
+        <v>700</v>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>766</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>765</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>212.22</v>
+      </c>
+      <c r="D124" t="n">
+        <v>211.3</v>
+      </c>
+      <c r="E124" t="n">
+        <v>209.83</v>
+      </c>
+      <c r="F124" t="n">
+        <v>208.79</v>
+      </c>
+      <c r="G124" t="n">
+        <v>25.85</v>
+      </c>
+      <c r="L124" t="n">
+        <v>700</v>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>767</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>766</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>212.89</v>
+      </c>
+      <c r="D125" t="n">
+        <v>212.22</v>
+      </c>
+      <c r="E125" t="n">
+        <v>210.98</v>
+      </c>
+      <c r="F125" t="n">
+        <v>209.83</v>
+      </c>
+      <c r="G125" t="n">
+        <v>30.92</v>
+      </c>
+      <c r="L125" t="n">
+        <v>500</v>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>768</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>767</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>214.55</v>
+      </c>
+      <c r="D126" t="n">
+        <v>212.89</v>
+      </c>
+      <c r="E126" t="n">
+        <v>212.03</v>
+      </c>
+      <c r="F126" t="n">
+        <v>210.98</v>
+      </c>
+      <c r="G126" t="n">
+        <v>17.35</v>
+      </c>
+      <c r="L126" t="n">
+        <v>250</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>767F</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>767</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>213.49</v>
+      </c>
+      <c r="D127" t="n">
+        <v>212.89</v>
+      </c>
+      <c r="E127" t="n">
+        <v>211.59</v>
+      </c>
+      <c r="F127" t="n">
+        <v>210.98</v>
+      </c>
+      <c r="G127" t="n">
+        <v>32.15</v>
+      </c>
+      <c r="L127" t="n">
+        <v>500</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>769</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>768</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>217.46</v>
+      </c>
+      <c r="D128" t="n">
+        <v>214.55</v>
+      </c>
+      <c r="E128" t="n">
+        <v>212.28</v>
+      </c>
+      <c r="F128" t="n">
+        <v>212.03</v>
+      </c>
+      <c r="G128" t="n">
+        <v>23.97</v>
+      </c>
+      <c r="L128" t="n">
+        <v>200</v>
+      </c>
+      <c r="W128" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>770</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>766</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>213.64</v>
+      </c>
+      <c r="D129" t="n">
+        <v>212.22</v>
+      </c>
+      <c r="E129" t="n">
+        <v>211.71</v>
+      </c>
+      <c r="F129" t="n">
+        <v>209.83</v>
+      </c>
+      <c r="G129" t="n">
+        <v>46.19</v>
+      </c>
+      <c r="L129" t="n">
+        <v>300</v>
+      </c>
+      <c r="W129" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="1048569" ht="12.8" customHeight="1" s="45"/>
     <row r="1048570" ht="12.8" customHeight="1" s="45"/>

</xml_diff>